<commit_message>
shadowing and finished pie charts
</commit_message>
<xml_diff>
--- a/Hours/research/files/research.xlsx
+++ b/Hours/research/files/research.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10768192\Desktop\pbischoff3.github.io\Hours\research\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23AA581-7CAD-4671-8613-BBF89DE2D67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF4EAAB-BD9B-4973-8794-C5A4FCDDAED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,13 @@
     <t>Hours</t>
   </si>
   <si>
-    <t>STEM</t>
-  </si>
-  <si>
     <t>Station1</t>
   </si>
   <si>
     <t>GCTx</t>
+  </si>
+  <si>
+    <t>S-STEM</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +386,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>89</v>
@@ -397,7 +397,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>270</v>
@@ -405,7 +405,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>110</v>

</xml_diff>